<commit_message>
Redo the spreadsheets for study 1, update manuscript, add qualtrics questions
</commit_message>
<xml_diff>
--- a/materials/study_01/anchor_babies.xlsx
+++ b/materials/study_01/anchor_babies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,18 +221,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -244,8 +236,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,7 +537,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,32 +554,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
@@ -591,30 +587,30 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13" t="str">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="str">
         <f>IF(D22=8,IFERROR(CONCATENATE("F(",E17,", ",E18,") = ",ROUND(E16, 2),", p ",IF(E19 &lt; 0.001, "&lt; .001", CONCATENATE("= ", ROUND(E19, 3)))), ""), "")</f>
         <v/>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="3" t="str">
         <f>IF(D22=8,IFERROR(IF(E19&lt;0.05,"✓", ""),""),"")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="str">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="str">
         <f>IF(D22=8,IFERROR(CONCATENATE("F(",D17,", ",D18,") = ",ROUND(D16,2),", p ",IF(D19 &lt; 0.001, "&lt; .001", CONCATENATE("= ", ROUND(D19, 3)))),""), "")</f>
         <v/>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="3" t="str">
         <f>IF(D22=8,IFERROR(IF(D19&gt;0.05,"✓", ""),""),"")</f>
         <v/>
@@ -623,25 +619,25 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13" t="str">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11" t="str">
         <f>IF(D22=8,IFERROR(CONCATENATE("F(",F17,", ",F18,") = ",ROUND(F16,2),", p ",IF(F19 &lt; 0.001, "&lt; .001", CONCATENATE("= ", ROUND(F19, 3)))),""),"")</f>
         <v/>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="3" t="str">
         <f>IF(D22=8,IFERROR(IF(F19&gt;0.05,"✓", ""),""),"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -656,48 +652,48 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -721,7 +717,7 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="e">
+      <c r="B16" s="6" t="e">
         <f>AVERAGE(D10,D12)</f>
         <v>#DIV/0!</v>
       </c>
@@ -745,7 +741,7 @@
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="8" t="e">
+      <c r="B17" s="6" t="e">
         <f>AVERAGE(D9,D11)</f>
         <v>#DIV/0!</v>
       </c>
@@ -769,22 +765,22 @@
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="8" t="e">
+      <c r="B18" s="6" t="e">
         <f>AVERAGE(D9,D10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <f>25+25+25+25-4</f>
         <v>96</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <f>25+25+25+25-4</f>
         <v>96</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <f>25+25+25+25-4</f>
         <v>96</v>
       </c>
@@ -793,7 +789,7 @@
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="8" t="e">
+      <c r="B19" s="6" t="e">
         <f>AVERAGE(D11,D12)</f>
         <v>#DIV/0!</v>
       </c>
@@ -856,11 +852,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D23">
-        <f>IF(D9="",0,1)</f>
+        <f t="shared" ref="D23:E26" si="0">IF(D9="",0,1)</f>
         <v>0</v>
       </c>
       <c r="E23">
-        <f>IF(E9="",0,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -873,11 +869,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D24">
-        <f>IF(D10="",0,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24">
-        <f>IF(E10="",0,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -890,11 +886,11 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <f>IF(D11="",0,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25">
-        <f>IF(E11="",0,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -907,11 +903,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D26">
-        <f>IF(D12="",0,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E26">
-        <f>IF(E12="",0,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -936,22 +932,22 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="16">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E6">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="✓">

</xml_diff>